<commit_message>
Updated Usokin benchmark results to include VAE models selected based on best reconstruction loss
</commit_message>
<xml_diff>
--- a/docs/Experiment 1 - Usokin/Benchmark Results.xlsx
+++ b/docs/Experiment 1 - Usokin/Benchmark Results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1327">
   <si>
     <t>model_name</t>
   </si>
@@ -3677,9 +3677,6 @@
     <t>AE</t>
   </si>
   <si>
-    <t>VAE</t>
-  </si>
-  <si>
     <t>UsokinVAE_BestTotalLoss</t>
   </si>
   <si>
@@ -3990,6 +3987,21 @@
   </si>
   <si>
     <t>adam:lr=3.864216798918698e-06</t>
+  </si>
+  <si>
+    <t>UsokinVAE_BestReconLoss</t>
+  </si>
+  <si>
+    <t>Dense:500:activation='tanh'|BatchNormalization|Dense:300:activation='tanh'|BatchNormalization</t>
+  </si>
+  <si>
+    <t>Dense:400:activation='elu'|BatchNormalization|Dense:350:activation='elu'|BatchNormalization|Dense:150:activation='elu'|BatchNormalization</t>
+  </si>
+  <si>
+    <t>VAE (Recon Loss)</t>
+  </si>
+  <si>
+    <t>VAE (Total Loss)</t>
   </si>
 </sst>
 </file>
@@ -4058,7 +4070,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4072,13 +4084,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4101,7 +4119,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4119,8 +4137,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4159,14 +4179,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -4174,6 +4199,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -4183,9 +4209,80 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4997,13 +5094,13 @@
         <v>86</v>
       </c>
       <c r="BM3" s="7" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="BN3" s="7">
         <v>10</v>
       </c>
       <c r="BO3" s="7" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="BP3" s="7">
         <v>25</v>
@@ -5191,13 +5288,13 @@
         <v>40</v>
       </c>
       <c r="BM4" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="BN4" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO4" s="1" t="s">
         <v>1270</v>
-      </c>
-      <c r="BN4" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO4" s="1" t="s">
-        <v>1271</v>
       </c>
       <c r="BP4" s="1">
         <v>25</v>
@@ -5385,13 +5482,13 @@
         <v>77</v>
       </c>
       <c r="BM5" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="BN5" s="1">
         <v>10</v>
       </c>
       <c r="BO5" s="1" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="BP5" s="1">
         <v>25</v>
@@ -5579,13 +5676,13 @@
         <v>96</v>
       </c>
       <c r="BM6" s="1" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="BN6" s="1">
         <v>15</v>
       </c>
       <c r="BO6" s="1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="BP6" s="1">
         <v>25</v>
@@ -5773,13 +5870,13 @@
         <v>63</v>
       </c>
       <c r="BM7" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="BN7" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO7" s="1" t="s">
         <v>1288</v>
-      </c>
-      <c r="BN7" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO7" s="1" t="s">
-        <v>1289</v>
       </c>
       <c r="BP7" s="1">
         <v>25</v>
@@ -5967,13 +6064,13 @@
         <v>100</v>
       </c>
       <c r="BM8" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="BN8" s="1">
         <v>20</v>
       </c>
       <c r="BO8" s="1" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="BP8" s="1">
         <v>10</v>
@@ -6161,13 +6258,13 @@
         <v>71</v>
       </c>
       <c r="BM9" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="BN9" s="1">
         <v>10</v>
       </c>
       <c r="BO9" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="BP9" s="1">
         <v>25</v>
@@ -6355,13 +6452,13 @@
         <v>65</v>
       </c>
       <c r="BM10" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="BN10" s="1">
         <v>25</v>
       </c>
       <c r="BO10" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="BP10" s="1">
         <v>25</v>
@@ -6549,13 +6646,13 @@
         <v>110</v>
       </c>
       <c r="BM11" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="BN11" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO11" s="1" t="s">
         <v>1318</v>
-      </c>
-      <c r="BN11" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO11" s="1" t="s">
-        <v>1319</v>
       </c>
       <c r="BP11" s="1">
         <v>10</v>
@@ -6743,13 +6840,13 @@
         <v>27</v>
       </c>
       <c r="BM12" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="BN12" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO12" s="1" t="s">
         <v>1258</v>
-      </c>
-      <c r="BN12" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO12" s="1" t="s">
-        <v>1259</v>
       </c>
       <c r="BP12" s="1">
         <v>25</v>
@@ -6937,13 +7034,13 @@
         <v>36</v>
       </c>
       <c r="BM13" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="BN13" s="1">
         <v>20</v>
       </c>
       <c r="BO13" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="BP13" s="1">
         <v>50</v>
@@ -7131,13 +7228,13 @@
         <v>69</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="BN14" s="1">
         <v>100</v>
       </c>
       <c r="BO14" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="BP14" s="1">
         <v>25</v>
@@ -7325,13 +7422,13 @@
         <v>67</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="BN15" s="1">
         <v>10</v>
       </c>
       <c r="BO15" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="BP15" s="1">
         <v>25</v>
@@ -7519,13 +7616,13 @@
         <v>55</v>
       </c>
       <c r="BM16" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="BN16" s="1">
         <v>25</v>
       </c>
       <c r="BO16" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="BP16" s="1">
         <v>25</v>
@@ -7713,13 +7810,13 @@
         <v>34</v>
       </c>
       <c r="BM17" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="BN17" s="1">
         <v>100</v>
       </c>
       <c r="BO17" s="1" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="BP17" s="1">
         <v>10</v>
@@ -7907,13 +8004,13 @@
         <v>46</v>
       </c>
       <c r="BM18" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="BN18" s="1">
         <v>10</v>
       </c>
       <c r="BO18" s="1" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="BP18" s="1">
         <v>10</v>
@@ -8101,13 +8198,13 @@
         <v>90</v>
       </c>
       <c r="BM19" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="BN19" s="1">
         <v>100</v>
       </c>
       <c r="BO19" s="1" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="BP19" s="1">
         <v>25</v>
@@ -8295,13 +8392,13 @@
         <v>94</v>
       </c>
       <c r="BM20" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="BN20" s="1">
         <v>200</v>
       </c>
       <c r="BO20" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="BP20" s="1">
         <v>10</v>
@@ -8489,13 +8586,13 @@
         <v>79</v>
       </c>
       <c r="BM21" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="BN21" s="1">
         <v>50</v>
       </c>
       <c r="BO21" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="BP21" s="1">
         <v>25</v>
@@ -8683,13 +8780,13 @@
         <v>104</v>
       </c>
       <c r="BM22" s="1" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="BN22" s="1">
         <v>100</v>
       </c>
       <c r="BO22" s="1" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="BP22" s="1">
         <v>25</v>
@@ -8877,13 +8974,13 @@
         <v>49</v>
       </c>
       <c r="BM23" s="1" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="BN23" s="1">
         <v>200</v>
       </c>
       <c r="BO23" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="BP23" s="1">
         <v>50</v>
@@ -9071,13 +9168,13 @@
         <v>57</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="BN24" s="1">
         <v>10</v>
       </c>
       <c r="BO24" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="BP24" s="1">
         <v>25</v>
@@ -9265,13 +9362,13 @@
         <v>84</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="BN25" s="1">
         <v>20</v>
       </c>
       <c r="BO25" s="1" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="BP25" s="1">
         <v>25</v>
@@ -9459,13 +9556,13 @@
         <v>14</v>
       </c>
       <c r="BM26" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="BN26" s="1">
         <v>15</v>
       </c>
       <c r="BO26" s="1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="BP26" s="1">
         <v>50</v>
@@ -9653,13 +9750,13 @@
         <v>53</v>
       </c>
       <c r="BM27" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="BN27" s="1">
         <v>15</v>
       </c>
       <c r="BO27" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="BP27" s="1">
         <v>10</v>
@@ -9847,13 +9944,13 @@
         <v>8</v>
       </c>
       <c r="BM28" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="BN28" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO28" s="1" t="s">
         <v>1244</v>
-      </c>
-      <c r="BN28" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO28" s="1" t="s">
-        <v>1245</v>
       </c>
       <c r="BP28" s="1">
         <v>50</v>
@@ -10041,13 +10138,13 @@
         <v>17</v>
       </c>
       <c r="BM29" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="BN29" s="1">
         <v>15</v>
       </c>
       <c r="BO29" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="BP29" s="1">
         <v>50</v>
@@ -10235,13 +10332,13 @@
         <v>112</v>
       </c>
       <c r="BM30" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="BN30" s="1">
         <v>15</v>
       </c>
       <c r="BO30" s="1" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="BP30" s="1">
         <v>50</v>
@@ -10429,13 +10526,13 @@
         <v>98</v>
       </c>
       <c r="BM31" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="BN31" s="1">
+        <v>25</v>
+      </c>
+      <c r="BO31" s="1" t="s">
         <v>1310</v>
-      </c>
-      <c r="BN31" s="1">
-        <v>25</v>
-      </c>
-      <c r="BO31" s="1" t="s">
-        <v>1311</v>
       </c>
       <c r="BP31" s="1">
         <v>25</v>
@@ -10623,13 +10720,13 @@
         <v>75</v>
       </c>
       <c r="BM32" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="BN32" s="1">
         <v>25</v>
       </c>
       <c r="BO32" s="1" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="BP32" s="1">
         <v>25</v>
@@ -10817,13 +10914,13 @@
         <v>61</v>
       </c>
       <c r="BM33" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="BN33" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO33" s="1" t="s">
         <v>1286</v>
-      </c>
-      <c r="BN33" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO33" s="1" t="s">
-        <v>1287</v>
       </c>
       <c r="BP33" s="1">
         <v>25</v>
@@ -11011,13 +11108,13 @@
         <v>51</v>
       </c>
       <c r="BM34" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="BN34" s="1">
         <v>15</v>
       </c>
       <c r="BO34" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="BP34" s="1">
         <v>50</v>
@@ -11205,13 +11302,13 @@
         <v>22</v>
       </c>
       <c r="BM35" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="BN35" s="1">
         <v>15</v>
       </c>
       <c r="BO35" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="BP35" s="1">
         <v>50</v>
@@ -11399,13 +11496,13 @@
         <v>59</v>
       </c>
       <c r="BM36" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="BN36" s="1">
         <v>10</v>
       </c>
       <c r="BO36" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="BP36" s="1">
         <v>25</v>
@@ -11593,13 +11690,13 @@
         <v>114</v>
       </c>
       <c r="BM37" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="BN37" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO37" s="1" t="s">
         <v>1321</v>
-      </c>
-      <c r="BN37" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO37" s="1" t="s">
-        <v>1322</v>
       </c>
       <c r="BP37" s="1">
         <v>25</v>
@@ -11787,13 +11884,13 @@
         <v>29</v>
       </c>
       <c r="BM38" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="BN38" s="1">
         <v>100</v>
       </c>
       <c r="BO38" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="BP38" s="1">
         <v>50</v>
@@ -11981,13 +12078,13 @@
         <v>108</v>
       </c>
       <c r="BM39" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="BN39" s="1">
         <v>200</v>
       </c>
       <c r="BO39" s="1" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="BP39" s="1">
         <v>50</v>
@@ -12175,13 +12272,13 @@
         <v>42</v>
       </c>
       <c r="BM40" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="BN40" s="1">
+        <v>50</v>
+      </c>
+      <c r="BO40" s="1" t="s">
         <v>1272</v>
-      </c>
-      <c r="BN40" s="1">
-        <v>50</v>
-      </c>
-      <c r="BO40" s="1" t="s">
-        <v>1273</v>
       </c>
       <c r="BP40" s="1">
         <v>50</v>
@@ -12369,13 +12466,13 @@
         <v>25</v>
       </c>
       <c r="BM41" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="BN41" s="1">
+        <v>50</v>
+      </c>
+      <c r="BO41" s="1" t="s">
         <v>1256</v>
-      </c>
-      <c r="BN41" s="1">
-        <v>50</v>
-      </c>
-      <c r="BO41" s="1" t="s">
-        <v>1257</v>
       </c>
       <c r="BP41" s="1">
         <v>50</v>
@@ -12563,13 +12660,13 @@
         <v>73</v>
       </c>
       <c r="BM42" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="BN42" s="1">
         <v>20</v>
       </c>
       <c r="BO42" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="BP42" s="1">
         <v>25</v>
@@ -12757,13 +12854,13 @@
         <v>106</v>
       </c>
       <c r="BM43" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="BN43" s="1">
         <v>50</v>
       </c>
       <c r="BO43" s="1" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="BP43" s="1">
         <v>25</v>
@@ -12951,13 +13048,13 @@
         <v>44</v>
       </c>
       <c r="BM44" s="1" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="BN44" s="1">
         <v>200</v>
       </c>
       <c r="BO44" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="BP44" s="1">
         <v>25</v>
@@ -13145,13 +13242,13 @@
         <v>19</v>
       </c>
       <c r="BM45" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="BN45" s="1">
         <v>20</v>
       </c>
       <c r="BO45" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="BP45" s="1">
         <v>10</v>
@@ -13339,13 +13436,13 @@
         <v>11</v>
       </c>
       <c r="BM46" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="BN46" s="1">
         <v>200</v>
       </c>
       <c r="BO46" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="BP46" s="1">
         <v>10</v>
@@ -13533,13 +13630,13 @@
         <v>88</v>
       </c>
       <c r="BM47" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="BN47" s="1">
+        <v>50</v>
+      </c>
+      <c r="BO47" s="1" t="s">
         <v>1303</v>
-      </c>
-      <c r="BN47" s="1">
-        <v>50</v>
-      </c>
-      <c r="BO47" s="1" t="s">
-        <v>1304</v>
       </c>
       <c r="BP47" s="1">
         <v>10</v>
@@ -13727,13 +13824,13 @@
         <v>102</v>
       </c>
       <c r="BM48" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="BN48" s="1">
         <v>10</v>
       </c>
       <c r="BO48" s="1" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="BP48" s="1">
         <v>50</v>
@@ -13921,13 +14018,13 @@
         <v>32</v>
       </c>
       <c r="BM49" s="1" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="BN49" s="1">
         <v>200</v>
       </c>
       <c r="BO49" s="1" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="BP49" s="1">
         <v>50</v>
@@ -14115,13 +14212,13 @@
         <v>38</v>
       </c>
       <c r="BM50" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="BN50" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO50" s="1" t="s">
         <v>1268</v>
-      </c>
-      <c r="BN50" s="1">
-        <v>10</v>
-      </c>
-      <c r="BO50" s="1" t="s">
-        <v>1269</v>
       </c>
       <c r="BP50" s="1">
         <v>10</v>
@@ -14303,13 +14400,13 @@
         <v>82</v>
       </c>
       <c r="BM51" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="BN51" s="1">
         <v>10</v>
       </c>
       <c r="BO51" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="BP51" s="1">
         <v>25</v>
@@ -14491,13 +14588,13 @@
         <v>92</v>
       </c>
       <c r="BM52" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="BN52" s="1">
         <v>10</v>
       </c>
       <c r="BO52" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="BP52" s="1">
         <v>25</v>
@@ -20335,21 +20432,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="18" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -20357,32 +20454,33 @@
     <col min="12" max="12" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>1243</v>
+      <c r="A1" s="3" t="s">
+        <v>1242</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1211</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1232</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>1233</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="17" t="s">
         <v>1234</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>1235</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>1236</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>1212</v>
@@ -20400,56 +20498,56 @@
         <v>1216</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>1217</v>
+      <c r="A2" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1325</v>
       </c>
       <c r="C2" s="2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+        <v>500</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>1223</v>
       </c>
       <c r="F2" s="2">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>739</v>
+        <v>15</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>232</v>
       </c>
       <c r="H2" s="2">
-        <v>10</v>
-      </c>
-      <c r="I2" s="13">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2">
         <v>4</v>
       </c>
       <c r="J2" s="2">
-        <v>0.135074120674568</v>
+        <v>8.9933775520242704E-2</v>
       </c>
       <c r="K2" s="2">
         <v>4</v>
       </c>
       <c r="L2" s="2">
-        <v>0.135074120674568</v>
+        <v>8.9933775520242704E-2</v>
       </c>
       <c r="M2" s="2">
-        <v>0.91494727900528205</v>
+        <v>0.95356096909127297</v>
       </c>
       <c r="N2" s="2">
-        <v>0.954983922829582</v>
+        <v>0.97588424437299004</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>1227</v>
+      <c r="A3" s="4" t="s">
+        <v>1226</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>1217</v>
@@ -20458,130 +20556,130 @@
         <v>100</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>1222</v>
       </c>
       <c r="F3" s="2">
-        <v>50</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>641</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>739</v>
       </c>
       <c r="H3" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I3" s="13">
         <v>4</v>
       </c>
       <c r="J3" s="2">
-        <v>9.60539737276771E-2</v>
+        <v>0.135074120674568</v>
       </c>
       <c r="K3" s="2">
         <v>4</v>
       </c>
       <c r="L3" s="2">
-        <v>9.60539737276771E-2</v>
+        <v>0.135074120674568</v>
       </c>
       <c r="M3" s="2">
-        <v>0.913584768652561</v>
+        <v>0.91494727900528205</v>
       </c>
       <c r="N3" s="2">
-        <v>0.95337620578778104</v>
+        <v>0.954983922829582</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="A4" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C4" s="2">
         <v>100</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F4" s="5">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="5">
-        <v>10</v>
-      </c>
-      <c r="I4" s="15">
-        <v>3</v>
-      </c>
-      <c r="J4" s="5">
-        <v>7.2106498000000005E-2</v>
-      </c>
-      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F4" s="2">
+        <v>50</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>641</v>
+      </c>
+      <c r="H4" s="2">
+        <v>25</v>
+      </c>
+      <c r="I4" s="13">
         <v>4</v>
       </c>
-      <c r="L4" s="5">
-        <v>0.230268574</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0.85109540900000002</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0.926045016</v>
+      <c r="J4" s="2">
+        <v>9.60539737276771E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9.60539737276771E-2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.913584768652561</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.95337620578778104</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C5" s="5">
-        <v>100</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F5" s="5">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="5">
-        <v>10</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="A5" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="5">
-        <v>0.158120654</v>
-      </c>
-      <c r="K5" s="5">
+      <c r="E5" s="4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F5" s="2">
+        <v>15</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="H5" s="2">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2">
+        <v>11</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.160222853917807</v>
+      </c>
+      <c r="K5" s="2">
         <v>4</v>
       </c>
-      <c r="L5" s="5">
-        <v>0.18788801399999999</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0.84440838600000001</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0.91961414799999996</v>
+      <c r="L5" s="2">
+        <v>0.18424799747321799</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.91357628195413898</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.95016077170418001</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>1227</v>
+      <c r="A6" s="4" t="s">
+        <v>1226</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>1217</v>
@@ -20592,13 +20690,13 @@
       <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>1231</v>
+      <c r="E6" s="4" t="s">
+        <v>1230</v>
       </c>
       <c r="F6" s="2">
         <v>50</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="18" t="s">
         <v>915</v>
       </c>
       <c r="H6" s="2">
@@ -20624,52 +20722,52 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>1217</v>
+      <c r="A7" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>1325</v>
       </c>
       <c r="C7" s="2">
-        <v>500</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1239</v>
+        <v>100</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1222</v>
       </c>
       <c r="F7" s="2">
-        <v>100</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>1240</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="H7" s="2">
         <v>10</v>
       </c>
-      <c r="I7" s="13">
-        <v>4</v>
+      <c r="I7" s="2">
+        <v>11</v>
       </c>
       <c r="J7" s="2">
-        <v>0.13751287985874899</v>
+        <v>0.16670032257897499</v>
       </c>
       <c r="K7" s="2">
         <v>4</v>
       </c>
       <c r="L7" s="2">
-        <v>0.13751287985874899</v>
+        <v>0.25341348618295401</v>
       </c>
       <c r="M7" s="2">
-        <v>0.88772186835671796</v>
+        <v>0.86899595632912896</v>
       </c>
       <c r="N7" s="2">
         <v>0.93569131832797403</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>1227</v>
+      <c r="A8" s="4" t="s">
+        <v>1226</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>1217</v>
@@ -20678,16 +20776,16 @@
         <v>500</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1224</v>
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1238</v>
       </c>
       <c r="F8" s="2">
-        <v>200</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>823</v>
+        <v>100</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>1239</v>
       </c>
       <c r="H8" s="2">
         <v>10</v>
@@ -20696,423 +20794,775 @@
         <v>4</v>
       </c>
       <c r="J8" s="2">
-        <v>3.5333530090974501E-2</v>
+        <v>0.13751287985874899</v>
       </c>
       <c r="K8" s="2">
         <v>4</v>
       </c>
       <c r="L8" s="2">
-        <v>3.5333530090974501E-2</v>
+        <v>0.13751287985874899</v>
       </c>
       <c r="M8" s="2">
-        <v>0.86435917210492497</v>
+        <v>0.88772186835671796</v>
       </c>
       <c r="N8" s="2">
-        <v>0.92443729903536997</v>
+        <v>0.93569131832797403</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="3" t="s">
         <v>1218</v>
       </c>
+      <c r="B9" s="20" t="s">
+        <v>1326</v>
+      </c>
       <c r="C9" s="5">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>1225</v>
+      <c r="E9" s="3" t="s">
+        <v>1220</v>
       </c>
       <c r="F9" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>296</v>
+        <v>504</v>
       </c>
       <c r="H9" s="5">
         <v>25</v>
       </c>
-      <c r="I9" s="13">
-        <v>4</v>
+      <c r="I9" s="5">
+        <v>11</v>
       </c>
       <c r="J9" s="5">
-        <v>0.10230879599999999</v>
+        <v>0.15745271299999999</v>
       </c>
       <c r="K9" s="5">
         <v>4</v>
       </c>
       <c r="L9" s="5">
-        <v>0.10230879599999999</v>
+        <v>0.16478970200000001</v>
       </c>
       <c r="M9" s="5">
-        <v>0.83225341900000005</v>
+        <v>0.87335470400000004</v>
       </c>
       <c r="N9" s="5">
-        <v>0.91318328000000004</v>
+        <v>0.92765273299999995</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="3" t="s">
         <v>1218</v>
       </c>
+      <c r="B10" s="20" t="s">
+        <v>1326</v>
+      </c>
       <c r="C10" s="5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1224</v>
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>1222</v>
       </c>
       <c r="F10" s="5">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>232</v>
+        <v>10</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="H10" s="5">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I10" s="15">
         <v>3</v>
       </c>
       <c r="J10" s="5">
-        <v>0.10967685100000001</v>
+        <v>7.2106498000000005E-2</v>
       </c>
       <c r="K10" s="5">
         <v>4</v>
       </c>
       <c r="L10" s="5">
-        <v>0.14447188699999999</v>
+        <v>0.230268574</v>
       </c>
       <c r="M10" s="5">
-        <v>0.83694743000000005</v>
+        <v>0.85109540900000002</v>
       </c>
       <c r="N10" s="5">
-        <v>0.91157556299999998</v>
+        <v>0.926045016</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="A11" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C11" s="2">
         <v>500</v>
       </c>
       <c r="D11" s="5">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F11" s="5">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="H11" s="5">
-        <v>10</v>
-      </c>
-      <c r="I11" s="15">
-        <v>11</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.16325188600000001</v>
-      </c>
-      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F11" s="2">
+        <v>200</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>823</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+      <c r="I11" s="13">
         <v>4</v>
       </c>
-      <c r="L11" s="5">
-        <v>0.18498842800000001</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0.83515199399999995</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0.90353697700000002</v>
+      <c r="J11" s="2">
+        <v>3.5333530090974501E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3.5333530090974501E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.86435917210492497</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.92443729903536997</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>1217</v>
+      <c r="A12" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>1325</v>
       </c>
       <c r="C12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D12" s="5">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1229</v>
+        <v>500</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1324</v>
       </c>
       <c r="F12" s="2">
-        <v>50</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>1089</v>
+        <v>15</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>392</v>
       </c>
       <c r="H12" s="2">
-        <v>25</v>
-      </c>
-      <c r="I12" s="13">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
+        <v>11</v>
       </c>
       <c r="J12" s="2">
-        <v>5.7272007083275102E-2</v>
+        <v>0.15081990980215501</v>
       </c>
       <c r="K12" s="2">
         <v>4</v>
       </c>
       <c r="L12" s="2">
-        <v>5.7272007083275102E-2</v>
+        <v>0.15092864428807401</v>
       </c>
       <c r="M12" s="2">
-        <v>0.84326704468595104</v>
+        <v>0.85704845786446804</v>
       </c>
       <c r="N12" s="2">
-        <v>0.91157556270096496</v>
+        <v>0.92282958199356901</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1000</v>
+      <c r="A13" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C13" s="5">
+        <v>100</v>
       </c>
       <c r="D13" s="5">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F13" s="2">
-        <v>200</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>1197</v>
-      </c>
-      <c r="H13" s="2">
-        <v>50</v>
-      </c>
-      <c r="I13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F13" s="5">
+        <v>20</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="5">
+        <v>10</v>
+      </c>
+      <c r="I13" s="15">
         <v>2</v>
       </c>
-      <c r="J13" s="2">
-        <v>1.0070884529153799E-2</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="J13" s="5">
+        <v>0.158120654</v>
+      </c>
+      <c r="K13" s="5">
         <v>4</v>
       </c>
-      <c r="L13" s="2">
-        <v>0.13898856216764799</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.79132191385843798</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0.88102893890675205</v>
+      <c r="L13" s="5">
+        <v>0.18788801399999999</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0.84440838600000001</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0.91961414799999996</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1000</v>
+      <c r="A14" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C14" s="5">
+        <v>500</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F14" s="2">
-        <v>500</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>1012</v>
-      </c>
-      <c r="H14" s="2">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F14" s="5">
+        <v>10</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="H14" s="5">
+        <v>25</v>
       </c>
       <c r="I14" s="13">
         <v>4</v>
       </c>
-      <c r="J14" s="2">
-        <v>6.0477085501550697E-2</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="J14" s="5">
+        <v>0.10230879599999999</v>
+      </c>
+      <c r="K14" s="5">
         <v>4</v>
       </c>
-      <c r="L14" s="2">
-        <v>6.0477085501550697E-2</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0.721460508014654</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.85209003215434098</v>
+      <c r="L14" s="5">
+        <v>0.10230879599999999</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0.83225341900000005</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0.91318328000000004</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="3" t="s">
         <v>1218</v>
       </c>
+      <c r="B15" s="20" t="s">
+        <v>1326</v>
+      </c>
       <c r="C15" s="5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F15" s="5">
+        <v>15</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H15" s="5">
+        <v>25</v>
+      </c>
+      <c r="I15" s="15">
         <v>3</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="F15" s="5">
-        <v>10</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>1242</v>
-      </c>
-      <c r="H15" s="5">
-        <v>25</v>
-      </c>
-      <c r="I15" s="13">
-        <v>4</v>
-      </c>
       <c r="J15" s="5">
-        <v>8.6785653000000004E-2</v>
+        <v>0.10967685100000001</v>
       </c>
       <c r="K15" s="5">
         <v>4</v>
       </c>
       <c r="L15" s="5">
-        <v>8.6785653000000004E-2</v>
+        <v>0.14447188699999999</v>
       </c>
       <c r="M15" s="5">
-        <v>0.82929916699999995</v>
+        <v>0.83694743000000005</v>
       </c>
       <c r="N15" s="5">
-        <v>0.90836012899999996</v>
+        <v>0.91157556299999998</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="A16" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C16" s="2">
         <v>1000</v>
       </c>
       <c r="D16" s="5">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F16" s="5">
-        <v>15</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="H16" s="5">
-        <v>25</v>
-      </c>
-      <c r="I16" s="15">
-        <v>11</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0.160062341</v>
-      </c>
-      <c r="K16" s="5">
+      <c r="E16" s="4" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F16" s="2">
+        <v>50</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H16" s="2">
+        <v>25</v>
+      </c>
+      <c r="I16" s="13">
         <v>4</v>
       </c>
-      <c r="L16" s="5">
-        <v>0.18744272000000001</v>
-      </c>
-      <c r="M16" s="5">
-        <v>0.70506883099999995</v>
-      </c>
-      <c r="N16" s="5">
-        <v>0.84244372999999995</v>
+      <c r="J16" s="2">
+        <v>5.7272007083275102E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>4</v>
+      </c>
+      <c r="L16" s="2">
+        <v>5.7272007083275102E-2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.84326704468595104</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.91157556270096496</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="3" t="s">
         <v>1218</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>1326</v>
       </c>
       <c r="C17" s="5">
         <v>1000</v>
       </c>
       <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1220</v>
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1240</v>
       </c>
       <c r="F17" s="5">
-        <v>20</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>451</v>
+        <v>10</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>1241</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
-      </c>
-      <c r="I17" s="15">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="I17" s="13">
+        <v>4</v>
       </c>
       <c r="J17" s="5">
-        <v>0.15964811400000001</v>
+        <v>8.6785653000000004E-2</v>
       </c>
       <c r="K17" s="5">
         <v>4</v>
       </c>
       <c r="L17" s="5">
+        <v>8.6785653000000004E-2</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0.82929916699999995</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0.90836012899999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C18" s="5">
+        <v>500</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F18" s="5">
+        <v>10</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="H18" s="5">
+        <v>10</v>
+      </c>
+      <c r="I18" s="15">
+        <v>11</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.16325188600000001</v>
+      </c>
+      <c r="K18" s="5">
+        <v>4</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0.18498842800000001</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0.83515199399999995</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.90353697700000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C19" s="2">
+        <v>500</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F19" s="2">
+        <v>20</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4.0941122864791298E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.18907373751495099</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.78693748846364697</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.887459807073955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C20" s="2">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F20" s="2">
+        <v>20</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.16317421853560499</v>
+      </c>
+      <c r="K20" s="2">
+        <v>4</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.16317421853560499</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.78162348175517904</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0.88424437299035397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F21" s="2">
+        <v>200</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H21" s="2">
+        <v>50</v>
+      </c>
+      <c r="I21" s="14">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.0070884529153799E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.13898856216764799</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.79132191385843798</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0.88102893890675205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H22" s="2">
+        <v>25</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4</v>
+      </c>
+      <c r="J22" s="2">
+        <v>9.2802294815436101E-2</v>
+      </c>
+      <c r="K22" s="2">
+        <v>4</v>
+      </c>
+      <c r="L22" s="2">
+        <v>9.2802294815436101E-2</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.77895645863858498</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0.87942122186495197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F23" s="2">
+        <v>500</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H23" s="2">
+        <v>50</v>
+      </c>
+      <c r="I23" s="13">
+        <v>4</v>
+      </c>
+      <c r="J23" s="2">
+        <v>6.0477085501550697E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <v>4</v>
+      </c>
+      <c r="L23" s="2">
+        <v>6.0477085501550697E-2</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.721460508014654</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.85209003215434098</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F24" s="2">
+        <v>20</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="H24" s="2">
+        <v>10</v>
+      </c>
+      <c r="I24" s="2">
+        <v>11</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.15850899130641899</v>
+      </c>
+      <c r="K24" s="2">
+        <v>4</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.305341969958215</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.53086786740395597</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0.80064308681672003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F25" s="5">
+        <v>20</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="H25" s="5">
+        <v>10</v>
+      </c>
+      <c r="I25" s="15">
+        <v>11</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.15964811400000001</v>
+      </c>
+      <c r="K25" s="5">
+        <v>4</v>
+      </c>
+      <c r="L25" s="5">
         <v>0.318395286</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M25" s="5">
         <v>0.51696761099999999</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N25" s="5">
         <v>0.76848874599999994</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N17">
-    <sortCondition ref="C10"/>
+  <sortState ref="A2:N25">
+    <sortCondition descending="1" ref="N1"/>
   </sortState>
-  <conditionalFormatting sqref="N2:N17">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="N2:N7 N9:N17">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -21123,7 +21573,53 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M17">
+  <conditionalFormatting sqref="M2:M7 M9:M17">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I7 I9:I17">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M7 M9:M25">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N7 N9:N25">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I7 I9:I25">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -21135,9 +21631,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>4</formula>
+  <conditionalFormatting sqref="M2:M25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed bug in AAE: added call to superclass's setup() method
</commit_message>
<xml_diff>
--- a/docs/Experiment 1 - Usokin/Benchmark Results.xlsx
+++ b/docs/Experiment 1 - Usokin/Benchmark Results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="1497">
   <si>
     <t>model_name</t>
   </si>
@@ -4245,6 +4245,273 @@
   </si>
   <si>
     <t>VAE=WarmUp (Total Loss)</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='tanh'", 'BatchNormalization', "Dense:250:activation='tanh'", 'BatchNormalization', "Dense:200:activation='tanh'", 'BatchNormalization', "Dense:10:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.9113250331983255e-05:momentum=0.9:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='sigmoid'", 'BatchNormalization', "Dense:300:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'", 'BatchNormalization', "Dense:15:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0002550271166160817</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='sigmoid'", 'BatchNormalization', "Dense:250:activation='sigmoid'", 'BatchNormalization', "Dense:150:activation='sigmoid'", 'BatchNormalization', "Dense:50:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=3.533289972020647e-05</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='elu'", 'BatchNormalization', "Dense:300:activation='elu'", 'BatchNormalization', "Dense:200:activation='elu'", 'BatchNormalization', "Dense:15:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=0.0002739417925180733:momentum=0.9:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=6.257179112409829e-05:momentum=0.99:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='tanh'", 'BatchNormalization', "Dense:350:activation='tanh'", 'BatchNormalization', "Dense:100:activation='tanh'", 'BatchNormalization', "Dense:100:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=1.1722352209612114e-07:momentum=0.9:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='tanh'", 'BatchNormalization', "Dense:350:activation='tanh'", 'BatchNormalization', "Dense:100:activation='tanh'", 'BatchNormalization', "Dense:50:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.129185309726257e-05:momentum=0.99:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='tanh'", 'BatchNormalization', "Dense:350:activation='tanh'", 'BatchNormalization', "Dense:200:activation='tanh'", 'BatchNormalization', "Dense:100:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.840226986106596e-05:momentum=0.5:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='tanh'", 'BatchNormalization', "Dense:250:activation='tanh'", 'BatchNormalization', "Dense:200:activation='tanh'", 'BatchNormalization', "Dense:25:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=3.717899064298368e-07:momentum=0.95:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:100:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0024475161969279473</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:200:activation='elu'", 'BatchNormalization', "Dense:20:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=1.499311703896513e-07:momentum=0.5:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='sigmoid'", 'BatchNormalization', "Dense:350:activation='sigmoid'", 'BatchNormalization', "Dense:200:activation='sigmoid'", 'BatchNormalization', "Dense:20:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.9783324536860215e-06:momentum=0.9:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='sigmoid'", 'BatchNormalization', "Dense:350:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.006810876935162646</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='relu'", 'BatchNormalization', "Dense:300:activation='relu'", 'BatchNormalization', "Dense:200:activation='relu'", 'BatchNormalization', "Dense:10:activation='relu'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=7.760518900091671e-05:momentum=0.5:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='sigmoid'", 'BatchNormalization', "Dense:250:activation='sigmoid'", 'BatchNormalization', "Dense:200:activation='sigmoid'", 'BatchNormalization', "Dense:20:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=0.00017432690465417434:momentum=0.5:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='sigmoid'", 'BatchNormalization', "Dense:350:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'", 'BatchNormalization', "Dense:50:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0035952879731740114</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='tanh'", 'BatchNormalization', "Dense:350:activation='tanh'", 'BatchNormalization', "Dense:100:activation='tanh'", 'BatchNormalization', "Dense:20:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=2.217465428823494e-05</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='relu'", 'BatchNormalization', "Dense:300:activation='relu'", 'BatchNormalization', "Dense:200:activation='relu'", 'BatchNormalization', "Dense:20:activation='relu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0002115207527084086</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='sigmoid'", 'BatchNormalization', "Dense:300:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'", 'BatchNormalization', "Dense:10:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=0.0005418286785727958:momentum=0.9:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='tanh'", 'BatchNormalization', "Dense:300:activation='tanh'", 'BatchNormalization', "Dense:150:activation='tanh'", 'BatchNormalization', "Dense:15:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0009124169832418194</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:100:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.007629841268919462</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0018401392460552066</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:100:activation='elu'", 'BatchNormalization', "Dense:25:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0015328584129431673</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0011317548256226432</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0007532644421392202</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:25:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=9.488513266672622e-05</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='relu'", 'BatchNormalization', "Dense:350:activation='relu'", 'BatchNormalization', "Dense:100:activation='relu'", 'BatchNormalization', "Dense:25:activation='relu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0018191829746738947</t>
+  </si>
+  <si>
+    <t>adam:lr=0.00045342970699985676</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:100:activation='elu'", 'BatchNormalization', "Dense:10:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.00413418816946174</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0018223199448585243</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='elu'", 'BatchNormalization', "Dense:350:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.009079877317427024</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='relu'", 'BatchNormalization', "Dense:250:activation='relu'", 'BatchNormalization', "Dense:150:activation='relu'", 'BatchNormalization', "Dense:50:activation='relu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0004403423985483893</t>
+  </si>
+  <si>
+    <t>adam:lr=0.00014896656536396818</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='elu'", 'BatchNormalization', "Dense:300:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:15:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0037253453995534694</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:50:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0006015845185189443</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0005840852180507002</t>
+  </si>
+  <si>
+    <t>adam:lr=9.783678629674962e-05</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:100:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=6.28328703075898e-05</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:15:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0003344682542372529</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='tanh'", 'BatchNormalization', "Dense:250:activation='tanh'", 'BatchNormalization', "Dense:150:activation='tanh'", 'BatchNormalization', "Dense:50:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0010977991811764191</t>
+  </si>
+  <si>
+    <t>adam:lr=0.0002619809875488492</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='relu'", 'BatchNormalization', "Dense:250:activation='relu'", 'BatchNormalization', "Dense:150:activation='relu'", 'BatchNormalization', "Dense:100:activation='relu'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.2501968116765985e-06:momentum=0.95:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='sigmoid'", 'BatchNormalization', "Dense:250:activation='sigmoid'", 'BatchNormalization', "Dense:150:activation='sigmoid'", 'BatchNormalization', "Dense:10:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=1.127026858406123e-05</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='tanh'", 'BatchNormalization', "Dense:300:activation='tanh'", 'BatchNormalization', "Dense:150:activation='tanh'", 'BatchNormalization', "Dense:50:activation='tanh'"]</t>
+  </si>
+  <si>
+    <t>sgd:lr=2.399229284858133e-06:momentum=0.95:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='elu'", 'BatchNormalization', "Dense:250:activation='elu'", 'BatchNormalization', "Dense:150:activation='elu'", 'BatchNormalization', "Dense:15:activation='elu'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.005633733536487037</t>
+  </si>
+  <si>
+    <t>sgd:lr=4.421320868400289e-07:momentum=0.99:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:400:activation='sigmoid'", 'BatchNormalization', "Dense:300:activation='sigmoid'", 'BatchNormalization', "Dense:200:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=0.00018231661537700767</t>
+  </si>
+  <si>
+    <t>["Dense:500:activation='sigmoid'", 'BatchNormalization', "Dense:300:activation='sigmoid'", 'BatchNormalization', "Dense:200:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'"]</t>
+  </si>
+  <si>
+    <t>adam:lr=4.1228962856564044e-05</t>
+  </si>
+  <si>
+    <t>sgd:lr=0.0008820875623419184:momentum=0.99:nesterov=True</t>
+  </si>
+  <si>
+    <t>["Dense:450:activation='sigmoid'", 'BatchNormalization', "Dense:300:activation='sigmoid'", 'BatchNormalization', "Dense:200:activation='sigmoid'", 'BatchNormalization', "Dense:100:activation='sigmoid'"]</t>
   </si>
 </sst>
 </file>
@@ -4398,7 +4665,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4417,6 +4684,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4490,7 +4759,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -4500,6 +4769,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -4511,6 +4781,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="17" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -4864,8 +5135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC52"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AG22" sqref="AG22"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16294,16 +16565,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="68.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="8" max="8" width="107.83203125" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="20" max="20" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="6" customFormat="1" ht="24" customHeight="1" thickBot="1">
@@ -16425,11 +16697,21 @@
       <c r="W2" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
+      <c r="Y2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>571</v>
+      </c>
       <c r="AE2" t="s">
         <v>0</v>
       </c>
@@ -16537,11 +16819,21 @@
       <c r="W3" s="7">
         <v>0.67565323099999997</v>
       </c>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+      <c r="Y3" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>0.690288283</v>
+      </c>
       <c r="AE3" s="8" t="s">
         <v>666</v>
       </c>
@@ -16649,11 +16941,21 @@
       <c r="W4" s="1">
         <v>0.67628484499999997</v>
       </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
+      <c r="Y4" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0.69052974899999997</v>
+      </c>
       <c r="AE4" t="s">
         <v>671</v>
       </c>
@@ -16761,11 +17063,21 @@
       <c r="W5" s="1">
         <v>0.676656174</v>
       </c>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
+      <c r="Y5" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0.69081305999999998</v>
+      </c>
       <c r="AE5" t="s">
         <v>662</v>
       </c>
@@ -16873,11 +17185,21 @@
       <c r="W6" s="1">
         <v>0.677029031</v>
       </c>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
+      <c r="Y6" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>1462</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0.69377672999999995</v>
+      </c>
       <c r="AE6" t="s">
         <v>658</v>
       </c>
@@ -16985,11 +17307,21 @@
       <c r="W7" s="1">
         <v>0.69026903299999998</v>
       </c>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
+      <c r="Y7" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0.70149834600000005</v>
+      </c>
       <c r="AE7" t="s">
         <v>668</v>
       </c>
@@ -17097,11 +17429,21 @@
       <c r="W8" s="1">
         <v>0.69653324699999997</v>
       </c>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
+      <c r="Y8" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0.70670385300000005</v>
+      </c>
       <c r="AE8" t="s">
         <v>692</v>
       </c>
@@ -17209,11 +17551,21 @@
       <c r="W9" s="1">
         <v>0.69789453400000001</v>
       </c>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
+      <c r="Y9" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0.70794852600000002</v>
+      </c>
       <c r="AE9" t="s">
         <v>646</v>
       </c>
@@ -17321,11 +17673,21 @@
       <c r="W10" s="1">
         <v>0.698063714</v>
       </c>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
+      <c r="Y10" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>1453</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0.70873285500000005</v>
+      </c>
       <c r="AE10" t="s">
         <v>638</v>
       </c>
@@ -17433,11 +17795,21 @@
       <c r="W11" s="1">
         <v>0.70029551800000001</v>
       </c>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
+      <c r="Y11" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0.711342951</v>
+      </c>
       <c r="AE11" t="s">
         <v>640</v>
       </c>
@@ -17545,11 +17917,21 @@
       <c r="W12" s="1">
         <v>0.700636068</v>
       </c>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
+      <c r="Y12" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0.71646480099999998</v>
+      </c>
       <c r="AE12" t="s">
         <v>632</v>
       </c>
@@ -17657,11 +18039,21 @@
       <c r="W13" s="1">
         <v>0.70104555999999996</v>
       </c>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
+      <c r="Y13" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0.71997550600000004</v>
+      </c>
       <c r="AE13" t="s">
         <v>649</v>
       </c>
@@ -17769,11 +18161,21 @@
       <c r="W14" s="1">
         <v>0.70280622000000004</v>
       </c>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
+      <c r="Y14" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>1438</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>0.72596689700000006</v>
+      </c>
       <c r="AE14" t="s">
         <v>679</v>
       </c>
@@ -17881,11 +18283,21 @@
       <c r="W15" s="1">
         <v>0.70497232499999996</v>
       </c>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
+      <c r="Y15" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>0.73369308600000005</v>
+      </c>
       <c r="AE15" t="s">
         <v>634</v>
       </c>
@@ -17993,11 +18405,21 @@
       <c r="W16" s="1">
         <v>0.70545596799999999</v>
       </c>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
+      <c r="Y16" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>0.73597605099999996</v>
+      </c>
       <c r="AE16" t="s">
         <v>654</v>
       </c>
@@ -18105,11 +18527,21 @@
       <c r="W17" s="1">
         <v>0.708218703</v>
       </c>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
+      <c r="Y17" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0.73715555600000005</v>
+      </c>
       <c r="AE17" t="s">
         <v>681</v>
       </c>
@@ -18217,11 +18649,21 @@
       <c r="W18" s="1">
         <v>0.70952962200000003</v>
       </c>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
+      <c r="Y18" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>1447</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>0.74097877499999998</v>
+      </c>
       <c r="AE18" t="s">
         <v>676</v>
       </c>
@@ -18329,11 +18771,21 @@
       <c r="W19" s="1">
         <v>0.71775917300000003</v>
       </c>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
+      <c r="Y19" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>0.75402836600000001</v>
+      </c>
       <c r="AE19" t="s">
         <v>622</v>
       </c>
@@ -18441,11 +18893,21 @@
       <c r="W20" s="1">
         <v>0.72024696300000002</v>
       </c>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
+      <c r="Y20" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>1462</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>0.75724078299999997</v>
+      </c>
       <c r="AE20" t="s">
         <v>660</v>
       </c>
@@ -18553,11 +19015,21 @@
       <c r="W21" s="1">
         <v>0.72918358999999999</v>
       </c>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
+      <c r="Y21" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0.76513940400000002</v>
+      </c>
       <c r="AE21" t="s">
         <v>651</v>
       </c>
@@ -18665,11 +19137,21 @@
       <c r="W22" s="1">
         <v>0.72937310799999999</v>
       </c>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
+      <c r="Y22" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0.78238860899999996</v>
+      </c>
       <c r="AE22" t="s">
         <v>644</v>
       </c>
@@ -18777,11 +19259,21 @@
       <c r="W23" s="1">
         <v>0.72955576099999997</v>
       </c>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
+      <c r="Y23" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0.78257406500000004</v>
+      </c>
       <c r="AE23" t="s">
         <v>642</v>
       </c>
@@ -18889,11 +19381,21 @@
       <c r="W24" s="1">
         <v>0.73693904200000004</v>
       </c>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
+      <c r="Y24" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>1412</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0.78569643</v>
+      </c>
       <c r="AE24" t="s">
         <v>636</v>
       </c>
@@ -19001,11 +19503,21 @@
       <c r="W25" s="1">
         <v>0.73924737299999999</v>
       </c>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
+      <c r="Y25" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0.79377020399999998</v>
+      </c>
       <c r="AE25" t="s">
         <v>683</v>
       </c>
@@ -19113,11 +19625,21 @@
       <c r="W26" s="1">
         <v>0.74976568600000004</v>
       </c>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
+      <c r="Y26" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>0.79578430200000005</v>
+      </c>
       <c r="AE26" t="s">
         <v>587</v>
       </c>
@@ -19225,11 +19747,21 @@
       <c r="W27" s="1">
         <v>0.75299645500000001</v>
       </c>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
+      <c r="Y27" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>0.79987264300000005</v>
+      </c>
       <c r="AE27" t="s">
         <v>664</v>
       </c>
@@ -19337,11 +19869,21 @@
       <c r="W28" s="1">
         <v>0.759303799</v>
       </c>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
+      <c r="Y28" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>0.80198178899999994</v>
+      </c>
       <c r="AE28" t="s">
         <v>630</v>
       </c>
@@ -19449,11 +19991,21 @@
       <c r="W29" s="1">
         <v>0.76089226600000004</v>
       </c>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
+      <c r="Y29" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>0.81016412100000001</v>
+      </c>
       <c r="AE29" t="s">
         <v>656</v>
       </c>
@@ -19561,11 +20113,21 @@
       <c r="W30" s="1">
         <v>0.77577659099999996</v>
       </c>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
+      <c r="Y30" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>0.84911320000000001</v>
+      </c>
       <c r="AE30" t="s">
         <v>605</v>
       </c>
@@ -19673,11 +20235,21 @@
       <c r="W31" s="1">
         <v>0.79565051200000003</v>
       </c>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
+      <c r="Y31" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>0.88408547500000001</v>
+      </c>
       <c r="AE31" t="s">
         <v>674</v>
       </c>
@@ -19785,11 +20357,21 @@
       <c r="W32" s="1">
         <v>0.81417365399999997</v>
       </c>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
+      <c r="Y32" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>0.90556935599999999</v>
+      </c>
       <c r="AE32" t="s">
         <v>593</v>
       </c>
@@ -19897,11 +20479,21 @@
       <c r="W33" s="1">
         <v>0.84175762399999998</v>
       </c>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
+      <c r="Y33" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>1443</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>0.96184949799999997</v>
+      </c>
       <c r="AE33" t="s">
         <v>581</v>
       </c>
@@ -20009,11 +20601,21 @@
       <c r="W34" s="1">
         <v>0.89481766699999998</v>
       </c>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
+      <c r="Y34" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>0.99724625899999997</v>
+      </c>
       <c r="AE34" t="s">
         <v>689</v>
       </c>
@@ -20121,11 +20723,21 @@
       <c r="W35" s="1">
         <v>0.93762869699999996</v>
       </c>
-      <c r="Y35" s="1"/>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="1"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="1"/>
+      <c r="Y35" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="AA35" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>1.0214041650000001</v>
+      </c>
       <c r="AE35" t="s">
         <v>602</v>
       </c>
@@ -20233,11 +20845,21 @@
       <c r="W36" s="1">
         <v>0.97847856899999996</v>
       </c>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1"/>
+      <c r="Y36" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>1.037520188</v>
+      </c>
       <c r="AE36" t="s">
         <v>611</v>
       </c>
@@ -20345,11 +20967,21 @@
       <c r="W37" s="1">
         <v>0.98745429299999998</v>
       </c>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
+      <c r="Y37" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>1.04656002</v>
+      </c>
       <c r="AE37" t="s">
         <v>584</v>
       </c>
@@ -20457,11 +21089,21 @@
       <c r="W38" s="1">
         <v>1.014566064</v>
       </c>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
+      <c r="Y38" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="AA38" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>1.103279495</v>
+      </c>
       <c r="AE38" t="s">
         <v>685</v>
       </c>
@@ -20569,11 +21211,21 @@
       <c r="W39" s="1">
         <v>1.0177118730000001</v>
       </c>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
+      <c r="Y39" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="Z39" s="1" t="s">
+        <v>1408</v>
+      </c>
+      <c r="AA39" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>1.11007677</v>
+      </c>
       <c r="AE39" t="s">
         <v>687</v>
       </c>
@@ -20681,11 +21333,21 @@
       <c r="W40" s="1">
         <v>1.0318004940000001</v>
       </c>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
+      <c r="Y40" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="Z40" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="AA40" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>1.135509487</v>
+      </c>
       <c r="AE40" t="s">
         <v>572</v>
       </c>
@@ -20793,11 +21455,21 @@
       <c r="W41" s="1">
         <v>1.0416702390000001</v>
       </c>
-      <c r="Y41" s="1"/>
-      <c r="Z41" s="1"/>
-      <c r="AA41" s="1"/>
-      <c r="AB41" s="1"/>
-      <c r="AC41" s="1"/>
+      <c r="Y41" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="Z41" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="AA41" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="AB41" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC41" s="1">
+        <v>1.167989666</v>
+      </c>
       <c r="AE41" t="s">
         <v>578</v>
       </c>
@@ -20905,11 +21577,21 @@
       <c r="W42" s="1">
         <v>1.057993806</v>
       </c>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
+      <c r="Y42" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z42" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="AA42" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC42" s="1">
+        <v>1.182257275</v>
+      </c>
       <c r="AE42" t="s">
         <v>613</v>
       </c>
@@ -21017,11 +21699,21 @@
       <c r="W43" s="1">
         <v>1.090644282</v>
       </c>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
+      <c r="Y43" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="Z43" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AA43" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>1.19271554</v>
+      </c>
       <c r="AE43" t="s">
         <v>627</v>
       </c>
@@ -21129,11 +21821,21 @@
       <c r="W44" s="1">
         <v>1.103089542</v>
       </c>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
+      <c r="Y44" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC44" s="1">
+        <v>1.19975692</v>
+      </c>
       <c r="AE44" t="s">
         <v>596</v>
       </c>
@@ -21241,11 +21943,21 @@
       <c r="W45" s="1">
         <v>1.1031509479999999</v>
       </c>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="1"/>
-      <c r="AA45" s="1"/>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="1"/>
+      <c r="Y45" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>1434</v>
+      </c>
+      <c r="AA45" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>1.2217608</v>
+      </c>
       <c r="AE45" t="s">
         <v>575</v>
       </c>
@@ -21353,11 +22065,21 @@
       <c r="W46" s="1">
         <v>1.1341237420000001</v>
       </c>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
-      <c r="AA46" s="1"/>
-      <c r="AB46" s="1"/>
-      <c r="AC46" s="1"/>
+      <c r="Y46" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>1414</v>
+      </c>
+      <c r="AA46" s="1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC46" s="1">
+        <v>1.2316023490000001</v>
+      </c>
       <c r="AE46" t="s">
         <v>608</v>
       </c>
@@ -21465,11 +22187,21 @@
       <c r="W47" s="1">
         <v>1.135845985</v>
       </c>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-      <c r="AA47" s="1"/>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
+      <c r="Y47" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="AA47" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>1.2324650260000001</v>
+      </c>
       <c r="AE47" t="s">
         <v>694</v>
       </c>
@@ -21577,11 +22309,21 @@
       <c r="W48" s="1">
         <v>1.173312887</v>
       </c>
-      <c r="Y48" s="1"/>
-      <c r="Z48" s="1"/>
-      <c r="AA48" s="1"/>
-      <c r="AB48" s="1"/>
-      <c r="AC48" s="1"/>
+      <c r="Y48" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="AA48" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC48" s="1">
+        <v>1.2354678560000001</v>
+      </c>
       <c r="AE48" t="s">
         <v>616</v>
       </c>
@@ -21689,11 +22431,21 @@
       <c r="W49" s="1">
         <v>1.197628906</v>
       </c>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
+      <c r="Y49" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z49" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="AA49" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC49" s="1">
+        <v>1.31272104</v>
+      </c>
       <c r="AE49" t="s">
         <v>590</v>
       </c>
@@ -21801,11 +22553,21 @@
       <c r="W50" s="1">
         <v>1.2396891759999999</v>
       </c>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-      <c r="AA50" s="1"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
+      <c r="Y50" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="Z50" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="AA50" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>1.3198193199999999</v>
+      </c>
       <c r="AE50" t="s">
         <v>625</v>
       </c>
@@ -21913,11 +22675,21 @@
       <c r="W51" s="1">
         <v>1.25551736</v>
       </c>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="1"/>
-      <c r="AA51" s="1"/>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="1"/>
+      <c r="Y51" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="AA51" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC51" s="1">
+        <v>1.465089176</v>
+      </c>
       <c r="AE51" t="s">
         <v>619</v>
       </c>
@@ -22025,11 +22797,21 @@
       <c r="W52" s="1">
         <v>1.268875325</v>
       </c>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
+      <c r="Y52" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC52" s="1">
+        <v>260.38049119999999</v>
+      </c>
       <c r="AE52" t="s">
         <v>599</v>
       </c>
@@ -22077,8 +22859,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="AQ3:AU52">
-    <sortCondition ref="AU2"/>
+  <sortState ref="Y3:AC52">
+    <sortCondition ref="AC2"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="AE1:AI1"/>
@@ -22091,6 +22873,7 @@
     <mergeCell ref="Y1:AC1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -22103,8 +22886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23:N30"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>